<commit_message>
Change some less common 500R resistors to 510R
</commit_message>
<xml_diff>
--- a/r4/build/bugg-main-r4-bom/bugg-main-r4.xlsx
+++ b/r4/build/bugg-main-r4-bom/bugg-main-r4.xlsx
@@ -682,7 +682,7 @@
     <t xml:space="preserve">R89, R98, </t>
   </si>
   <si>
-    <t xml:space="preserve">500R</t>
+    <t xml:space="preserve">510R</t>
   </si>
   <si>
     <t xml:space="preserve">R9, R10, R90, </t>
@@ -1189,11 +1189,11 @@
   </sheetPr>
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="82:82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.05"/>
@@ -1532,6 +1532,9 @@
       <c r="B17" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="C17" s="2" t="n">
+        <v>4</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Remove NP0 constraint from 10nF 50V caps. The only instance that could have demanded NP0 is the 15V DCDC,  ut its eval board BOM uses X7R's.
</commit_message>
<xml_diff>
--- a/r4/build/bugg-main-r4-bom/bugg-main-r4.xlsx
+++ b/r4/build/bugg-main-r4-bom/bugg-main-r4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="330">
   <si>
     <t xml:space="preserve">Ref</t>
   </si>
@@ -1189,8 +1189,8 @@
   </sheetPr>
   <dimension ref="A1:K116"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A82" activeCellId="0" sqref="82:82"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1515,9 +1515,6 @@
       <c r="F16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="I16" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>